<commit_message>
initial commit2. last one lacking data file
</commit_message>
<xml_diff>
--- a/data/Stdev-sheet_unprotected.xlsx
+++ b/data/Stdev-sheet_unprotected.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ohsuitg-my.sharepoint.com/personal/morgansc_ohsu_edu/Documents/Catherine Morgans/Duvoisin and Morgans Labs/Melanoma project/Projects/MAR_project/23-03/QAH-DED_analysis_e1-359/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ohsuitg-my.sharepoint.com/personal/morgansc_ohsu_edu/Documents/Catherine Morgans/Duvoisin and Morgans Labs/Melanoma project/Projects/MAR_project/Figures_analysis/cytokine array/QAH-DED_analysis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="4" documentId="8_{7EC3818D-71CA-404E-B313-57461F68A5B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EDAF19F3-DD77-2F48-B452-B06A0E510D95}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="2300" windowWidth="27240" windowHeight="16440" activeTab="1" xr2:uid="{185BE1F4-4432-7440-A7EE-7EF2C34EDA82}"/>
+    <workbookView xWindow="1560" yWindow="2300" windowWidth="27240" windowHeight="16440" xr2:uid="{185BE1F4-4432-7440-A7EE-7EF2C34EDA82}"/>
   </bookViews>
   <sheets>
     <sheet name="Stdev_linear-reg" sheetId="1" r:id="rId1"/>
@@ -1970,6 +1970,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2271,8 +2275,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7087E61-5F06-BE4E-BC79-5CAA27648DEC}">
   <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:I1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3478,7 +3482,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{903D04DD-D8F3-934D-BBFD-1DC28C4F02BE}">
   <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1:I1048576"/>
     </sheetView>
   </sheetViews>

</xml_diff>